<commit_message>
SUM two static numbers
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC57FEA-74B4-9648-AFA9-6C7FDFC19F78}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD000789-F228-744A-980B-8B174DA092BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26380" yWindow="3820" windowWidth="24240" windowHeight="14920" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SUM</t>
   </si>
@@ -33,15 +33,6 @@
     <t>inputs</t>
   </si>
   <si>
-    <t>=SUM(B2,C2,D2)</t>
-  </si>
-  <si>
-    <t>=SUM(B2:D2)</t>
-  </si>
-  <si>
-    <t>=SUM(B2,C2:D2)</t>
-  </si>
-  <si>
     <t>0 PARAM FUNCTIONS</t>
   </si>
   <si>
@@ -52,6 +43,18 @@
   </si>
   <si>
     <t>=SUM(1,2)</t>
+  </si>
+  <si>
+    <t>=SUM(B4)</t>
+  </si>
+  <si>
+    <t>=SUM(B4,C4,D4)</t>
+  </si>
+  <si>
+    <t>=SUM(B4:D4)</t>
+  </si>
+  <si>
+    <t>=SUM(B4,C4:D4)</t>
   </si>
 </sst>
 </file>
@@ -99,12 +102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -434,7 +438,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -443,11 +447,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43234.615911805558</v>
+        <v>43234.636556712961</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -476,7 +480,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <f>SUM(1)</f>
@@ -485,7 +489,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <f>SUM(1,2)</f>
@@ -494,27 +498,36 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <f>SUM(B4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <f>SUM(B4,C4,D4)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <f>SUM(B4:D4)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <f>SUM(B4,C4:D4)</f>
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Resolved cell.formula into $$("Sheet!A1")
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD000789-F228-744A-980B-8B174DA092BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B60ED7-8FD9-6D41-9BB7-AA8A0CB4CAA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26380" yWindow="3820" windowWidth="24240" windowHeight="14920" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
+    <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>SUM</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>=SUM(B4,C4:D4)</t>
+  </si>
+  <si>
+    <t>SUM of 1st degree referential params</t>
+  </si>
+  <si>
+    <t>=SUM(B5)</t>
+  </si>
+  <si>
+    <t>=SUM(B5, B6)</t>
+  </si>
+  <si>
+    <t>=SUM(B5,B6,B7,B8)</t>
   </si>
 </sst>
 </file>
@@ -102,13 +114,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -434,36 +447,43 @@
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="4.5546875" customWidth="1"/>
+    <col min="5" max="5" width="1.44140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43234.636556712961</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43235.427235185183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -476,9 +496,8 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -486,8 +505,15 @@
         <f>SUM(1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <f>SUM(B5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -495,8 +521,15 @@
         <f>SUM(1,2)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <f>SUM(B5, B6)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -505,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -513,8 +546,15 @@
         <f>SUM(B4,C4,D4)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B5,B6,B7,B8)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -523,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Resolved multiple cell.formula into $$("Sheet!A1"), $$("Sheet!A2")
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B60ED7-8FD9-6D41-9BB7-AA8A0CB4CAA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBDCFF5-CF61-6A43-BC02-9E1026FBC478}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Evaluate references to ranges with formula
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6F4B9D-47CC-2C4D-8A54-F3371CF8C787}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1805D8F-2E50-5943-99DE-5569DC01C710}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="NOW">Sheet1!$F$24</definedName>
+    <definedName name="SUM">Sheet1!$F$23</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>SUM</t>
   </si>
@@ -85,6 +89,12 @@
   </si>
   <si>
     <t>=SUM(SUM(1), B5)</t>
+  </si>
+  <si>
+    <t>=SUM(B5:B8)</t>
+  </si>
+  <si>
+    <t>=SUM(B8,B9:B10)</t>
   </si>
 </sst>
 </file>
@@ -454,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F23" sqref="F23:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -468,6 +478,7 @@
     <col min="5" max="5" width="1.44140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="4.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -484,7 +495,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43235.625073958334</v>
+        <v>43237.663700810182</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -580,6 +591,13 @@
         <f>SUM(B4:D4)</f>
         <v>6</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f>SUM(B5:B8)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -589,6 +607,13 @@
         <f>SUM(B4,C4:D4)</f>
         <v>6</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <f>SUM(B8,B9:B10)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -639,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -648,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -656,6 +681,12 @@
         <f>SUM(SUM(1), B5)</f>
         <v>2</v>
       </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented custom fun definition serialization Implemented unary node visitor
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4544785-1164-9D4D-9102-4960AA199CC2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCAE802-11CE-CA43-9D63-E81E35AB9FBC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-16080" windowWidth="21600" windowHeight="37940" activeTab="1" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
+    <workbookView xWindow="33600" yWindow="6100" windowWidth="21600" windowHeight="14900" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="NOW">Sheet1!$F$24</definedName>
-    <definedName name="SUM">Sheet1!$F$23</definedName>
+    <definedName name="NOW">Sheet1!$F$23</definedName>
+    <definedName name="SUM">Sheet1!$F$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>SUM</t>
   </si>
@@ -119,7 +119,22 @@
     <t>=SUM(B2,B3)</t>
   </si>
   <si>
-    <t>STATIC FIELD</t>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>STATIC FIELD 1</t>
+  </si>
+  <si>
+    <t>STATIC FIELD 2</t>
+  </si>
+  <si>
+    <t>STATIC FIELD 3</t>
+  </si>
+  <si>
+    <t>STATIC FIELD 4</t>
+  </si>
+  <si>
+    <t>static fields</t>
   </si>
 </sst>
 </file>
@@ -143,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +183,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -195,6 +216,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,13 +533,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="4.5546875" customWidth="1"/>
     <col min="5" max="5" width="1.44140625" style="6" customWidth="1"/>
@@ -540,7 +562,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43238.410173379627</v>
+        <v>43240.430766782411</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -727,8 +749,100 @@
         <v>2</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="13">
+        <v>10</v>
+      </c>
+      <c r="C22" s="13">
+        <v>20</v>
+      </c>
+      <c r="D22" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="13">
+        <v>100</v>
+      </c>
+      <c r="C23" s="13">
+        <v>200</v>
+      </c>
+      <c r="D23" s="13">
+        <v>300</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F24" s="3"/>
+      <c r="A24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B25)</f>
+        <v>=MATCH($B$24,$B$21:$B$23,0)</v>
+      </c>
+      <c r="B25">
+        <f>MATCH($B$24,$B$21:$B$23,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f t="shared" ref="A26:A27" ca="1" si="0">_xlfn.FORMULATEXT(B26)</f>
+        <v>=MATCH($B$24,$B$21:$B$23,1)</v>
+      </c>
+      <c r="B26">
+        <f>MATCH($B$24,$B$21:$B$23,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MATCH($B$24,$B$21:$B$23,-1)</v>
+      </c>
+      <c r="B27">
+        <f>MATCH($B$24,$B$21:$B$23,-1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H30" s="3"/>
@@ -741,15 +855,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AD45B1-F440-6C49-8277-3732F9B5BF93}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -768,7 +882,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -812,7 +926,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="11">
         <v>5</v>
@@ -822,22 +936,34 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11">
+        <v>50</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11">
+        <v>500</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="11">
+        <v>5000</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -856,7 +982,7 @@
       </c>
       <c r="B13" s="6">
         <f>SUM(B2)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -867,12 +993,51 @@
       </c>
       <c r="B14" s="6">
         <f>SUM(B2,B3)</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B21)</f>
+        <v>=MATCH(B2,$B$7:$B$10,0)</v>
+      </c>
+      <c r="B21">
+        <f>MATCH(B2,$B$7:$B$10,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f t="shared" ref="A22:A23" ca="1" si="0">_xlfn.FORMULATEXT(B22)</f>
+        <v>=MATCH(B2,$B$7:$B$10,1)</v>
+      </c>
+      <c r="B22">
+        <f>MATCH(B2,$B$7:$B$10,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MATCH(B2,$B$7:$B$10,-1)</v>
+      </c>
+      <c r="B23">
+        <f>MATCH(B2,$B$7:$B$10,-1)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue with current sheet when accessing ranges
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD56E6-6498-6D4D-ADEB-880BFD176392}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A8BAB5-CCBF-D04E-84EC-B7979390CA06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="6100" windowWidth="21600" windowHeight="14900" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -547,7 +547,7 @@
     <col min="3" max="4" width="4.5546875" customWidth="1"/>
     <col min="5" max="5" width="1.44140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -565,7 +565,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43240.63707488426</v>
+        <v>43240.836198726851</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -683,6 +683,16 @@
       <c r="G10">
         <f>SUM(B8,B9:B10)</f>
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F11" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G11)</f>
+        <v>=SUM(Sheet2!B7:B10)</v>
+      </c>
+      <c r="G11">
+        <f>SUM(Sheet2!B7:B10)</f>
+        <v>5555</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -999,7 +1009,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cell may now return error
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A8BAB5-CCBF-D04E-84EC-B7979390CA06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8687FCC6-2BBF-F947-B69D-9BC1569DBB45}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="6100" windowWidth="21600" windowHeight="14900" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
+    <workbookView xWindow="6000" yWindow="6100" windowWidth="21600" windowHeight="14900" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43240.836198726851</v>
+        <v>43242.918370717591</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -887,8 +887,9 @@
       <c r="B31" s="13">
         <v>10</v>
       </c>
-      <c r="C31" s="13">
-        <v>20</v>
+      <c r="C31" s="13" t="e">
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
       </c>
       <c r="D31" s="13">
         <v>30</v>

</xml_diff>

<commit_message>
Persist null members in array (#28)
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8687FCC6-2BBF-F947-B69D-9BC1569DBB45}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC3BE4-70C1-E049-A4F5-4EA55D016E5D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="6100" windowWidth="21600" windowHeight="14900" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
+    <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="BadSheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="NOW">Sheet1!$F$23</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>SUM</t>
   </si>
@@ -138,13 +139,22 @@
   </si>
   <si>
     <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>Range with holes</t>
+  </si>
+  <si>
+    <t>README: THIS IS A BAD SHEET TO DEMONSTRATE FAULT TOLERANCE AND ERROR RESISTANCE</t>
+  </si>
+  <si>
+    <t>RANGE EVALUATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="18"/>
       <color theme="1"/>
@@ -156,6 +166,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -220,6 +238,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -565,7 +586,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43242.918370717591</v>
+        <v>43243.622310069448</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1192,4 +1213,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51EF42E-6BD5-374B-88DB-90A249D2E7C9}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B9)</f>
+        <v>=SUM(B4:C6)</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B4:C6)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B10)</f>
+        <v>=VLOOKUP(0,$B$4:$C$6,2,0)</v>
+      </c>
+      <c r="B10" t="e">
+        <f>VLOOKUP(0,$B$4:$C$6,2,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B11)</f>
+        <v>=VLOOKUP(2,$B$4:$C$6,2,0)</v>
+      </c>
+      <c r="B11">
+        <f>VLOOKUP(2,$B$4:$C$6,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B12)</f>
+        <v>=VLOOKUP(3,$B$4:$C$6,2,0)</v>
+      </c>
+      <c r="B12">
+        <f>VLOOKUP(3,$B$4:$C$6,2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Supports upto 702 columns A -> ZZ
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC3BE4-70C1-E049-A4F5-4EA55D016E5D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6049B04F-C2AE-7740-A863-340B436437FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <definedName name="SUM">Sheet1!$F$22</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>SUM</t>
   </si>
@@ -148,6 +149,9 @@
   </si>
   <si>
     <t>RANGE EVALUATION</t>
+  </si>
+  <si>
+    <t>MORE CONTENTS ARE AVAILABLE BEYOND "AA" COLUMN</t>
   </si>
 </sst>
 </file>
@@ -179,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -223,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -241,6 +251,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -570,26 +582,33 @@
     <col min="6" max="6" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43243.622310069448</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>43244.642694097223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,8 +621,14 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -616,8 +641,20 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -632,8 +669,15 @@
         <f>SUM(B5)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <f>SUM(1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -648,8 +692,15 @@
         <f>SUM(B5, B6)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB6">
+        <f>SUM(1,2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -657,8 +708,15 @@
         <f>SUM(B4)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB7" s="5">
+        <f>SUM(AB4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,8 +731,15 @@
         <f>SUM(B5,B6,B7,B8)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB8">
+        <f>SUM(AB4,AC4,AD4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -689,8 +754,15 @@
         <f>SUM(B5:B8)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9">
+        <f>SUM(AB4:AD4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -705,8 +777,15 @@
         <f>SUM(B8,B9:B10)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AA10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB10">
+        <f>SUM(AB4,AC4:AD4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="F11" t="str">
         <f ca="1">_xlfn.FORMULATEXT(G11)</f>
         <v>=SUM(Sheet2!B7:B10)</v>
@@ -716,7 +795,7 @@
         <v>5555</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -724,7 +803,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -738,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -747,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -756,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Added fun INDEX implementation
</commit_message>
<xml_diff>
--- a/sample/test.xlsx
+++ b/sample/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khanhhua/dev/formula1js/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6049B04F-C2AE-7740-A863-340B436437FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C60B46-70A9-8146-A6EC-9230A4E07492}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-16940" windowWidth="21600" windowHeight="37940" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
+    <workbookView xWindow="12000" yWindow="460" windowWidth="21600" windowHeight="20540" xr2:uid="{73998C74-935A-454D-AE3A-14CBDBF148F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>SUM</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>MORE CONTENTS ARE AVAILABLE BEYOND "AA" COLUMN</t>
+  </si>
+  <si>
+    <t>INDEX</t>
   </si>
 </sst>
 </file>
@@ -248,11 +251,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B3B35B-3790-464F-8B55-E314074DAD3E}">
-  <dimension ref="A1:AD41"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -592,12 +595,12 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -605,7 +608,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">NOW()</f>
-        <v>43244.642694097223</v>
+        <v>43245.293408217593</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -1009,7 +1012,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" ref="A33:A40" ca="1" si="1">_xlfn.FORMULATEXT(B33)</f>
         <v>=VLOOKUP(0,$B$30:$D$32,3,FALSE())</v>
@@ -1019,7 +1022,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(1,$B$30:$D$32,3,FALSE())</v>
@@ -1029,7 +1032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(2,$B$30:$D$32,3,FALSE())</v>
@@ -1039,7 +1042,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(10,$B$30:$D$32,3,FALSE())</v>
@@ -1049,7 +1052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(0,$B$30:$D$32,3,TRUE())</v>
@@ -1059,7 +1062,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(1,$B$30:$D$32,3,TRUE())</v>
@@ -1069,7 +1072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(2,$B$30:$D$32,3,TRUE())</v>
@@ -1079,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=VLOOKUP(10,$B$30:$D$32,3,TRUE())</v>
@@ -1089,7 +1092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" ref="A41" ca="1" si="2">_xlfn.FORMULATEXT(B41)</f>
         <v>=VLOOKUP(101,$B$30:$D$32,3,TRUE())</v>
@@ -1097,6 +1100,126 @@
       <c r="B41">
         <f>VLOOKUP(101,$B$30:$D$32,3,TRUE())</f>
         <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="13">
+        <v>1</v>
+      </c>
+      <c r="C44" s="13">
+        <v>2</v>
+      </c>
+      <c r="D44" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="13">
+        <v>10</v>
+      </c>
+      <c r="C45" s="13">
+        <v>20</v>
+      </c>
+      <c r="D45" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="13">
+        <v>100</v>
+      </c>
+      <c r="C46" s="13">
+        <v>200</v>
+      </c>
+      <c r="D46" s="13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f t="shared" ref="A47:A53" ca="1" si="3">_xlfn.FORMULATEXT(B47)</f>
+        <v>=INDEX($B$44:$D$44,0)</v>
+      </c>
+      <c r="B47">
+        <f>INDEX($B$44:$D$44,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$D$44,1)</v>
+      </c>
+      <c r="B48">
+        <f>INDEX($B$44:$D$44,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$D$44,2)</v>
+      </c>
+      <c r="B49">
+        <f>INDEX($B$44:$D$44,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$B$46,1)</v>
+      </c>
+      <c r="B50">
+        <f>INDEX($B$44:$B$46,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$B$46,2)</v>
+      </c>
+      <c r="B51">
+        <f>INDEX($B$44:$B$46,2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$D$46,1)</v>
+      </c>
+      <c r="B52" t="e">
+        <f>INDEX($B$44:$D$46,1)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=INDEX($B$44:$D$46,2)</v>
+      </c>
+      <c r="B53" t="e">
+        <f>INDEX($B$44:$D$46,2)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -1308,16 +1431,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">

</xml_diff>